<commit_message>
DiagramaBN v1.0 oficial 16.10.24
</commit_message>
<xml_diff>
--- a/CCapsTools/ES2N - Requisitos Funcionais v3.0.xlsx
+++ b/CCapsTools/ES2N - Requisitos Funcionais v3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\GitHub Denilce\ES2\CCapsTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1644DD95-A487-4EC8-8DDC-2C08A19969DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D7DA98-D622-4878-8759-163EE4FBA939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4ABF0B59-3EAA-4472-9014-1459B26A9A3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -799,10 +799,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -810,107 +807,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1006,6 +902,107 @@
           <color indexed="64"/>
         </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1084,12 +1081,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE4463AF-6EFD-417D-87F3-CCC089358462}" name="Tabela1" displayName="Tabela1" ref="A7:F24" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A7:F24" xr:uid="{CE4463AF-6EFD-417D-87F3-CCC089358462}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8D0A53C3-30EE-4630-8AF6-A892EE5E66D0}" name="Código" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{87B05248-128B-467D-8485-990498FF2EDD}" name="Nome" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{80A49610-4FD2-484C-9CB4-05978882901C}" name="Descrição" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F7EE7D55-1316-4B00-B421-506813E6E0AA}" name="Nível de Acesso_x000a_(Tipos de acesso: Aluno, Administrador, Instrutor/Palestrante e Comissão)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{83D1078F-DAB6-4986-AD6A-767F20C7AA1A}" name="Prioridade (Alta,_x000a_Média, Baixa)" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{1864F1CA-2EDD-4018-AA15-2A517F1C747C}" name="Requisito(s) que é  (são)_x000a_executado(s) ou pode(m)_x000a_ser executado(s) na sequência" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{8D0A53C3-30EE-4630-8AF6-A892EE5E66D0}" name="Código" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{87B05248-128B-467D-8485-990498FF2EDD}" name="Nome" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{80A49610-4FD2-484C-9CB4-05978882901C}" name="Descrição" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F7EE7D55-1316-4B00-B421-506813E6E0AA}" name="Nível de Acesso_x000a_(Tipos de acesso: Aluno, Administrador, Instrutor/Palestrante e Comissão)" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{83D1078F-DAB6-4986-AD6A-767F20C7AA1A}" name="Prioridade (Alta,_x000a_Média, Baixa)" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1864F1CA-2EDD-4018-AA15-2A517F1C747C}" name="Requisito(s) que é  (são)_x000a_executado(s) ou pode(m)_x000a_ser executado(s) na sequência" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1394,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3837308E-2BE3-4051-9282-618B7392BE50}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,7 +1461,7 @@
       <c r="A8" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1484,7 +1481,7 @@
       <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1504,7 +1501,7 @@
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1524,7 +1521,7 @@
       <c r="A11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1542,7 +1539,7 @@
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1560,7 +1557,7 @@
       <c r="A13" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1580,7 +1577,7 @@
       <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1600,7 +1597,7 @@
       <c r="A15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1620,7 +1617,7 @@
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="10" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1640,7 +1637,7 @@
       <c r="A17" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1658,7 +1655,7 @@
       <c r="A18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="10" t="s">
         <v>61</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1678,7 +1675,7 @@
       <c r="A19" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1698,7 +1695,7 @@
       <c r="A20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="11" t="s">
@@ -1718,7 +1715,7 @@
       <c r="A21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -1736,7 +1733,7 @@
       <c r="A22" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="10" t="s">
         <v>82</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -1752,7 +1749,7 @@
       <c r="A23" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>79</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -1766,7 +1763,7 @@
       <c r="A24" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1793,9 +1790,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1913,25 +1913,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1953,9 +1943,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9030A888-F94C-446A-AE50-538902A00351}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9386896A-91B6-4EC7-AC94-350129FCA8CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>